<commit_message>
Implementing damage charts for different unit sizes, refactoring codebase
</commit_message>
<xml_diff>
--- a/data/starcraft_damages.xlsx
+++ b/data/starcraft_damages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\Projects\StarcraftDamageGraphs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861A0061-5789-4DCB-A84E-C2882C7FABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495CD6F7-D79F-4EAF-B070-3880BA45321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13320" yWindow="750" windowWidth="15480" windowHeight="14850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terran" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1358,7 +1358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899E6C49-E106-4BA9-A1ED-379D0F6B6235}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1962,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Implementing damage calculation logic, adding new feature for graphs
</commit_message>
<xml_diff>
--- a/data/starcraft_damages.xlsx
+++ b/data/starcraft_damages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\Projects\StarcraftDamageGraphs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495CD6F7-D79F-4EAF-B070-3880BA45321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768CEF9A-916F-44CA-97A2-845A48F90A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="750" windowWidth="15480" windowHeight="14850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13320" yWindow="750" windowWidth="15480" windowHeight="14850" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terran" sheetId="1" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>Air Attack Mod</t>
   </si>
   <si>
-    <t>Air/Ground</t>
-  </si>
-  <si>
     <t>ground</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Shield Armor</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -619,13 +621,13 @@
         <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -669,7 +671,7 @@
         <v>24</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -713,7 +715,7 @@
         <v>24</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -757,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -801,7 +803,7 @@
         <v>24</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -845,7 +847,7 @@
         <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -889,7 +891,7 @@
         <v>24</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -933,7 +935,7 @@
         <v>24</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -977,7 +979,7 @@
         <v>25</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1021,7 +1023,7 @@
         <v>24</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1065,7 +1067,7 @@
         <v>24</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1109,7 +1111,7 @@
         <v>24</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1153,7 +1155,7 @@
         <v>25</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1197,7 +1199,7 @@
         <v>24</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1241,12 +1243,12 @@
         <v>24</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -1285,7 +1287,7 @@
         <v>24</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1358,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899E6C49-E106-4BA9-A1ED-379D0F6B6235}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,19 +1405,19 @@
         <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -1454,13 +1456,13 @@
         <v>24</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
@@ -1499,13 +1501,13 @@
         <v>24</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
@@ -1544,13 +1546,13 @@
         <v>24</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>23</v>
@@ -1589,13 +1591,13 @@
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -1634,13 +1636,13 @@
         <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -1679,13 +1681,13 @@
         <v>24</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -1724,13 +1726,13 @@
         <v>25</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -1769,13 +1771,13 @@
         <v>25</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -1814,13 +1816,13 @@
         <v>24</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -1859,13 +1861,13 @@
         <v>24</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -1904,13 +1906,13 @@
         <v>25</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -1949,13 +1951,13 @@
         <v>24</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
@@ -1994,13 +1996,13 @@
         <v>24</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
@@ -2039,13 +2041,13 @@
         <v>24</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -2084,7 +2086,7 @@
         <v>24</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -2159,6 +2161,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2166,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813B1AA2-0C49-4602-9A0A-7EB5E6BA6B07}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,18 +2218,18 @@
         <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -2265,12 +2268,12 @@
         <v>24</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
@@ -2309,12 +2312,12 @@
         <v>24</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -2353,12 +2356,12 @@
         <v>24</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
@@ -2397,12 +2400,12 @@
         <v>24</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
@@ -2441,12 +2444,12 @@
         <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -2485,12 +2488,12 @@
         <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -2529,12 +2532,12 @@
         <v>24</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -2573,12 +2576,12 @@
         <v>25</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -2617,12 +2620,12 @@
         <v>24</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -2661,12 +2664,12 @@
         <v>24</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -2705,12 +2708,12 @@
         <v>24</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -2749,12 +2752,12 @@
         <v>25</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
@@ -2793,12 +2796,12 @@
         <v>24</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
@@ -2837,12 +2840,12 @@
         <v>24</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -2881,7 +2884,7 @@
         <v>24</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>